<commit_message>
fixed nike ticker to nke
</commit_message>
<xml_diff>
--- a/ticker-examples.xlsx
+++ b/ticker-examples.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reginaclarke/Mandalorians/Unit_1/Project1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reginaclarke/Mandalorians/Unit_1/Project1/The-Retail-Bootcamp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47778E30-254D-1142-AB37-9A6C13473887}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41402B4-8BE3-784E-9BF5-14182C5C2DBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="3900" windowWidth="28040" windowHeight="15940" xr2:uid="{9914FF46-D102-9448-8A07-723C744D22DD}"/>
+    <workbookView xWindow="60" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{9914FF46-D102-9448-8A07-723C744D22DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>M</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>COMPANY NAME</t>
+  </si>
+  <si>
+    <t>NKE</t>
   </si>
 </sst>
 </file>
@@ -592,7 +595,7 @@
   <dimension ref="F9:G23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -660,7 +663,7 @@
     </row>
     <row r="17" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F17" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
reduced number of example tickers to use based on the user testing; will need to add disclaimer regarding data source; this will be continued post mvp work.
</commit_message>
<xml_diff>
--- a/ticker-examples.xlsx
+++ b/ticker-examples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reginaclarke/Mandalorians/Unit_1/Project1/The-Retail-Bootcamp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41402B4-8BE3-784E-9BF5-14182C5C2DBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5113BE-DBAE-AC40-AF3D-6E047F909475}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{9914FF46-D102-9448-8A07-723C744D22DD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>M</t>
   </si>
@@ -41,36 +41,6 @@
     <t>MACY'S</t>
   </si>
   <si>
-    <t>LB</t>
-  </si>
-  <si>
-    <t>L BRANDS</t>
-  </si>
-  <si>
-    <t>AEO</t>
-  </si>
-  <si>
-    <t>AMERICAN EAGLE OUTFITTERS</t>
-  </si>
-  <si>
-    <t>FL</t>
-  </si>
-  <si>
-    <t>FOOT LOCKER</t>
-  </si>
-  <si>
-    <t>JWN</t>
-  </si>
-  <si>
-    <t>NORDSTROM</t>
-  </si>
-  <si>
-    <t>GPS</t>
-  </si>
-  <si>
-    <t>THE GAP</t>
-  </si>
-  <si>
     <t>ROST</t>
   </si>
   <si>
@@ -83,25 +53,7 @@
     <t>BURLINGTON STORES</t>
   </si>
   <si>
-    <t>PVH</t>
-  </si>
-  <si>
-    <t>PHILLIP VAN HUSSEN (CK, TOMMY H, ETC)</t>
-  </si>
-  <si>
-    <t>RL</t>
-  </si>
-  <si>
-    <t>RALPH LAUREN</t>
-  </si>
-  <si>
     <t>NIKE</t>
-  </si>
-  <si>
-    <t>GIL</t>
-  </si>
-  <si>
-    <t>GILDAN ACTIVEWEAR</t>
   </si>
   <si>
     <t>TICKER</t>
@@ -592,25 +544,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B57B6DEC-F1C9-6C44-9700-882F18F9453A}">
-  <dimension ref="F9:G23"/>
+  <dimension ref="F9:G15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="6" max="6" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="9" spans="6:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="6:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="F10" s="2" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="6:7" x14ac:dyDescent="0.2">
@@ -623,96 +575,32 @@
     </row>
     <row r="12" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F12" s="4" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="14" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>22</v>
+    <row r="14" spans="6:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="15" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F16" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F17" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="6:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F22" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="6:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="6:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F11:G22">
-    <sortCondition ref="G11:G22"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F11:G14">
+    <sortCondition ref="G11:G14"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>